<commit_message>
Minor additions heavy on xslx
</commit_message>
<xml_diff>
--- a/NHLplayers.xlsx
+++ b/NHLplayers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benca\Documents\HockeySim\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E70E709-376A-48F4-A893-37BC3BBB6616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12D72E-AEA7-44DB-A1C5-505AF2FD895B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CF0E87D5-685B-476C-95EB-D2A8834F4C8B}"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="11460" windowHeight="9960" xr2:uid="{CF0E87D5-685B-476C-95EB-D2A8834F4C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="1" r:id="rId1"/>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECDA566-A1CB-4F29-BEF9-B661E32BA4DF}">
   <dimension ref="A1:AI93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6678,6 +6678,9 @@
       <c r="M48">
         <v>82</v>
       </c>
+      <c r="N48">
+        <v>90</v>
+      </c>
       <c r="O48">
         <v>78</v>
       </c>
@@ -6715,15 +6718,15 @@
       </c>
       <c r="Y48">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>70.040000000000006</v>
+        <v>88.04</v>
       </c>
       <c r="Z48">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>62.960000000000008</v>
+        <v>80.960000000000008</v>
       </c>
       <c r="AA48">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>68.64</v>
+        <v>86.64</v>
       </c>
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
@@ -6768,6 +6771,9 @@
       <c r="M49">
         <v>94</v>
       </c>
+      <c r="N49">
+        <v>97</v>
+      </c>
       <c r="O49">
         <v>79</v>
       </c>
@@ -6805,15 +6811,15 @@
       </c>
       <c r="Y49">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>69.92</v>
+        <v>89.320000000000007</v>
       </c>
       <c r="Z49">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>66.12</v>
+        <v>85.52000000000001</v>
       </c>
       <c r="AA49">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>70.64</v>
+        <v>90.04</v>
       </c>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
@@ -6858,6 +6864,9 @@
       <c r="M50">
         <v>87</v>
       </c>
+      <c r="N50">
+        <v>97</v>
+      </c>
       <c r="O50">
         <v>85</v>
       </c>
@@ -6895,15 +6904,15 @@
       </c>
       <c r="Y50">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>68.239999999999995</v>
+        <v>87.64</v>
       </c>
       <c r="Z50">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67</v>
+        <v>86.4</v>
       </c>
       <c r="AA50">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.559999999999988</v>
+        <v>86.96</v>
       </c>
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
@@ -6948,6 +6957,9 @@
       <c r="M51">
         <v>91</v>
       </c>
+      <c r="N51">
+        <v>93</v>
+      </c>
       <c r="O51">
         <v>78</v>
       </c>
@@ -6985,15 +6997,15 @@
       </c>
       <c r="Y51">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>67.560000000000016</v>
+        <v>86.160000000000025</v>
       </c>
       <c r="Z51">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.12</v>
+        <v>82.72</v>
       </c>
       <c r="AA51">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.28</v>
+        <v>85.88</v>
       </c>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
@@ -7038,6 +7050,9 @@
       <c r="M52">
         <v>82</v>
       </c>
+      <c r="N52">
+        <v>87</v>
+      </c>
       <c r="O52">
         <v>82</v>
       </c>
@@ -7075,15 +7090,15 @@
       </c>
       <c r="Y52">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>66</v>
+        <v>83.4</v>
       </c>
       <c r="Z52">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>65.28</v>
+        <v>82.68</v>
       </c>
       <c r="AA52">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>66.559999999999988</v>
+        <v>83.96</v>
       </c>
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
@@ -7128,6 +7143,9 @@
       <c r="M53">
         <v>80</v>
       </c>
+      <c r="N53">
+        <v>87</v>
+      </c>
       <c r="O53">
         <v>83</v>
       </c>
@@ -7165,15 +7183,15 @@
       </c>
       <c r="Y53">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>65</v>
+        <v>82.4</v>
       </c>
       <c r="Z53">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.400000000000006</v>
+        <v>84.800000000000011</v>
       </c>
       <c r="AA53">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>65.2</v>
+        <v>82.600000000000009</v>
       </c>
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
@@ -7218,6 +7236,9 @@
       <c r="M54">
         <v>82</v>
       </c>
+      <c r="N54">
+        <v>81</v>
+      </c>
       <c r="O54">
         <v>70</v>
       </c>
@@ -7255,15 +7276,15 @@
       </c>
       <c r="Y54">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>66.11999999999999</v>
+        <v>82.32</v>
       </c>
       <c r="Z54">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>57.56</v>
+        <v>73.760000000000005</v>
       </c>
       <c r="AA54">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.92</v>
+        <v>81.12</v>
       </c>
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
@@ -7308,6 +7329,9 @@
       <c r="M55">
         <v>91</v>
       </c>
+      <c r="N55">
+        <v>83</v>
+      </c>
       <c r="O55">
         <v>78</v>
       </c>
@@ -7345,15 +7369,15 @@
       </c>
       <c r="Y55">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>68</v>
+        <v>84.6</v>
       </c>
       <c r="Z55">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.36</v>
+        <v>80.960000000000008</v>
       </c>
       <c r="AA55">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>68.16</v>
+        <v>84.759999999999991</v>
       </c>
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
@@ -7398,6 +7422,9 @@
       <c r="M56">
         <v>84</v>
       </c>
+      <c r="N56">
+        <v>96</v>
+      </c>
       <c r="O56">
         <v>80</v>
       </c>
@@ -7435,15 +7462,15 @@
       </c>
       <c r="Y56">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>64.440000000000012</v>
+        <v>83.640000000000015</v>
       </c>
       <c r="Z56">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.400000000000006</v>
+        <v>83.600000000000009</v>
       </c>
       <c r="AA56">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.160000000000011</v>
+        <v>83.360000000000014</v>
       </c>
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
@@ -7488,6 +7515,9 @@
       <c r="M57">
         <v>82</v>
       </c>
+      <c r="N57">
+        <v>84</v>
+      </c>
       <c r="O57">
         <v>83</v>
       </c>
@@ -7525,15 +7555,15 @@
       </c>
       <c r="Y57">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>64.600000000000009</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="Z57">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.8</v>
+        <v>84.6</v>
       </c>
       <c r="AA57">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.08</v>
+        <v>80.88</v>
       </c>
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
@@ -7578,6 +7608,9 @@
       <c r="M58">
         <v>82</v>
       </c>
+      <c r="N58">
+        <v>90</v>
+      </c>
       <c r="O58">
         <v>82</v>
       </c>
@@ -7615,15 +7648,15 @@
       </c>
       <c r="Y58">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>64.92</v>
+        <v>82.92</v>
       </c>
       <c r="Z58">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.959999999999994</v>
+        <v>82.96</v>
       </c>
       <c r="AA58">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>65.52000000000001</v>
+        <v>83.52000000000001</v>
       </c>
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
@@ -7668,6 +7701,9 @@
       <c r="M59">
         <v>78</v>
       </c>
+      <c r="N59">
+        <v>77</v>
+      </c>
       <c r="O59">
         <v>84</v>
       </c>
@@ -7705,15 +7741,15 @@
       </c>
       <c r="Y59">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>63.64</v>
+        <v>79.040000000000006</v>
       </c>
       <c r="Z59">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>68.92</v>
+        <v>84.320000000000007</v>
       </c>
       <c r="AA59">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>63.400000000000006</v>
+        <v>78.800000000000011</v>
       </c>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
@@ -7758,6 +7794,9 @@
       <c r="M60">
         <v>87</v>
       </c>
+      <c r="N60">
+        <v>99</v>
+      </c>
       <c r="O60">
         <v>90</v>
       </c>
@@ -7795,15 +7834,15 @@
       </c>
       <c r="Y60">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>68.44</v>
+        <v>88.24</v>
       </c>
       <c r="Z60">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>70.88</v>
+        <v>90.679999999999993</v>
       </c>
       <c r="AA60">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.56</v>
+        <v>87.36</v>
       </c>
       <c r="AB60" s="1"/>
       <c r="AC60" s="1"/>
@@ -7848,6 +7887,9 @@
       <c r="M61">
         <v>90</v>
       </c>
+      <c r="N61">
+        <v>92</v>
+      </c>
       <c r="O61">
         <v>85</v>
       </c>
@@ -7885,15 +7927,15 @@
       </c>
       <c r="Y61">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>70.280000000000015</v>
+        <v>88.680000000000021</v>
       </c>
       <c r="Z61">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.56</v>
+        <v>85.960000000000008</v>
       </c>
       <c r="AA61">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>69.52000000000001</v>
+        <v>87.920000000000016</v>
       </c>
       <c r="AB61" s="1"/>
       <c r="AC61" s="1"/>
@@ -7938,6 +7980,9 @@
       <c r="M62">
         <v>77</v>
       </c>
+      <c r="N62">
+        <v>88</v>
+      </c>
       <c r="O62">
         <v>93</v>
       </c>
@@ -7975,15 +8020,15 @@
       </c>
       <c r="Y62">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>63.480000000000011</v>
+        <v>81.080000000000013</v>
       </c>
       <c r="Z62">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>71.84</v>
+        <v>89.44</v>
       </c>
       <c r="AA62">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>63.68</v>
+        <v>81.28</v>
       </c>
       <c r="AB62" s="1"/>
       <c r="AC62" s="1"/>
@@ -8028,6 +8073,9 @@
       <c r="M63">
         <v>83</v>
       </c>
+      <c r="N63">
+        <v>92</v>
+      </c>
       <c r="O63">
         <v>84</v>
       </c>
@@ -8065,15 +8113,15 @@
       </c>
       <c r="Y63">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>64.720000000000013</v>
+        <v>83.120000000000019</v>
       </c>
       <c r="Z63">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>66.48</v>
+        <v>84.88000000000001</v>
       </c>
       <c r="AA63">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>64.36</v>
+        <v>82.76</v>
       </c>
       <c r="AB63" s="1"/>
       <c r="AC63" s="1"/>
@@ -8118,6 +8166,9 @@
       <c r="M64">
         <v>82</v>
       </c>
+      <c r="N64">
+        <v>84</v>
+      </c>
       <c r="O64">
         <v>86</v>
       </c>
@@ -8155,15 +8206,15 @@
       </c>
       <c r="Y64">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>66.12</v>
+        <v>82.92</v>
       </c>
       <c r="Z64">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>68.12</v>
+        <v>84.92</v>
       </c>
       <c r="AA64">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>65.08</v>
+        <v>81.88</v>
       </c>
       <c r="AB64" s="1"/>
       <c r="AC64" s="1"/>
@@ -8208,6 +8259,9 @@
       <c r="M65">
         <v>70</v>
       </c>
+      <c r="N65">
+        <v>84</v>
+      </c>
       <c r="O65">
         <v>87</v>
       </c>
@@ -8245,15 +8299,15 @@
       </c>
       <c r="Y65">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>58.960000000000008</v>
+        <v>75.760000000000005</v>
       </c>
       <c r="Z65">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>67.959999999999994</v>
+        <v>84.759999999999991</v>
       </c>
       <c r="AA65">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>59.280000000000008</v>
+        <v>76.080000000000013</v>
       </c>
       <c r="AB65" s="1"/>
       <c r="AC65" s="1"/>
@@ -8298,6 +8352,9 @@
       <c r="M66">
         <v>12</v>
       </c>
+      <c r="N66">
+        <v>94</v>
+      </c>
       <c r="O66">
         <v>12</v>
       </c>
@@ -8335,15 +8392,15 @@
       </c>
       <c r="Y66">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>9.6000000000000014</v>
+        <v>28.400000000000002</v>
       </c>
       <c r="Z66">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.6000000000000014</v>
+        <v>28.400000000000002</v>
       </c>
       <c r="AA66">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.5999999999999979</v>
+        <v>28.4</v>
       </c>
       <c r="AB66" s="1"/>
       <c r="AC66" s="1"/>
@@ -8388,6 +8445,9 @@
       <c r="M67">
         <v>12</v>
       </c>
+      <c r="N67">
+        <v>80</v>
+      </c>
       <c r="O67">
         <v>12</v>
       </c>
@@ -8425,15 +8485,15 @@
       </c>
       <c r="Y67">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>9.6000000000000014</v>
+        <v>25.6</v>
       </c>
       <c r="Z67">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.6000000000000014</v>
+        <v>25.6</v>
       </c>
       <c r="AA67">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.5999999999999979</v>
+        <v>25.599999999999998</v>
       </c>
       <c r="AB67" s="1"/>
       <c r="AC67" s="1"/>
@@ -8478,6 +8538,9 @@
       <c r="M68">
         <v>80</v>
       </c>
+      <c r="N68">
+        <v>82</v>
+      </c>
       <c r="O68">
         <v>77</v>
       </c>
@@ -8515,15 +8578,15 @@
       </c>
       <c r="Y68">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>62.400000000000006</v>
+        <v>78.800000000000011</v>
       </c>
       <c r="Z68">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>61.08</v>
+        <v>77.48</v>
       </c>
       <c r="AA68">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>61.84</v>
+        <v>78.240000000000009</v>
       </c>
       <c r="AB68" s="1"/>
       <c r="AC68" s="1"/>
@@ -8568,6 +8631,9 @@
       <c r="M69">
         <v>72</v>
       </c>
+      <c r="N69">
+        <v>79</v>
+      </c>
       <c r="O69">
         <v>83</v>
       </c>
@@ -8605,15 +8671,15 @@
       </c>
       <c r="Y69">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>57.2</v>
+        <v>73</v>
       </c>
       <c r="Z69">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>65.92</v>
+        <v>81.72</v>
       </c>
       <c r="AA69">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>57.48</v>
+        <v>73.28</v>
       </c>
       <c r="AB69" s="1"/>
       <c r="AC69" s="1"/>
@@ -8658,6 +8724,9 @@
       <c r="M70">
         <v>75</v>
       </c>
+      <c r="N70">
+        <v>78</v>
+      </c>
       <c r="O70">
         <v>77</v>
       </c>
@@ -8695,15 +8764,15 @@
       </c>
       <c r="Y70">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>60.760000000000005</v>
+        <v>76.360000000000014</v>
       </c>
       <c r="Z70">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>63.08</v>
+        <v>78.680000000000007</v>
       </c>
       <c r="AA70">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>60.68</v>
+        <v>76.28</v>
       </c>
       <c r="AB70" s="1"/>
       <c r="AC70" s="1"/>

</xml_diff>

<commit_message>
Fixed recursive error in counting shots/goals
</commit_message>
<xml_diff>
--- a/NHLplayers.xlsx
+++ b/NHLplayers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benca\Documents\HockeySim\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12D72E-AEA7-44DB-A1C5-505AF2FD895B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27A7C23-AA9E-4A3B-A96F-40FE9E3366EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="11460" windowHeight="9960" xr2:uid="{CF0E87D5-685B-476C-95EB-D2A8834F4C8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CF0E87D5-685B-476C-95EB-D2A8834F4C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="1" r:id="rId1"/>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECDA566-A1CB-4F29-BEF9-B661E32BA4DF}">
   <dimension ref="A1:AI93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" topLeftCell="G66" workbookViewId="0">
+      <selection activeCell="Y91" sqref="Y91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8811,40 +8811,61 @@
       <c r="I71">
         <v>1</v>
       </c>
+      <c r="L71">
+        <v>84</v>
+      </c>
+      <c r="M71">
+        <v>97</v>
+      </c>
+      <c r="N71">
+        <v>99</v>
+      </c>
+      <c r="O71">
+        <v>84</v>
+      </c>
+      <c r="P71">
+        <v>86</v>
+      </c>
+      <c r="Q71">
+        <v>93</v>
+      </c>
+      <c r="R71">
+        <v>12</v>
+      </c>
       <c r="S71">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="T71">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="U71">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="V71">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="W71">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X71">
         <v>50</v>
       </c>
       <c r="Y71">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>91.4</v>
       </c>
       <c r="Z71">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>88.44</v>
       </c>
       <c r="AA71">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>91.6</v>
       </c>
       <c r="AB71" s="1"/>
       <c r="AC71" s="1"/>
@@ -8883,40 +8904,61 @@
       <c r="I72">
         <v>1</v>
       </c>
+      <c r="L72">
+        <v>97</v>
+      </c>
+      <c r="M72">
+        <v>88</v>
+      </c>
+      <c r="N72">
+        <v>94</v>
+      </c>
+      <c r="O72">
+        <v>82</v>
+      </c>
+      <c r="P72">
+        <v>78</v>
+      </c>
+      <c r="Q72">
+        <v>77</v>
+      </c>
+      <c r="R72">
+        <v>12</v>
+      </c>
       <c r="S72">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="T72">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="U72">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="V72">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="W72">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X72">
         <v>50</v>
       </c>
       <c r="Y72">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>90.64</v>
       </c>
       <c r="Z72">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>84.679999999999993</v>
       </c>
       <c r="AA72">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>89.4</v>
       </c>
       <c r="AB72" s="1"/>
       <c r="AC72" s="1"/>
@@ -8955,40 +8997,61 @@
       <c r="I73">
         <v>1</v>
       </c>
+      <c r="L73">
+        <v>81</v>
+      </c>
+      <c r="M73">
+        <v>83</v>
+      </c>
+      <c r="N73">
+        <v>91</v>
+      </c>
+      <c r="O73">
+        <v>89</v>
+      </c>
+      <c r="P73">
+        <v>90</v>
+      </c>
+      <c r="Q73">
+        <v>86</v>
+      </c>
+      <c r="R73">
+        <v>12</v>
+      </c>
       <c r="S73">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="T73">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="U73">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="V73">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="W73">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X73">
         <v>50</v>
       </c>
       <c r="Y73">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>85.04000000000002</v>
       </c>
       <c r="Z73">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>88.800000000000011</v>
       </c>
       <c r="AA73">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>85.36</v>
       </c>
       <c r="AB73" s="1"/>
       <c r="AC73" s="1"/>
@@ -9027,40 +9090,61 @@
       <c r="I74">
         <v>2</v>
       </c>
+      <c r="L74">
+        <v>83</v>
+      </c>
+      <c r="M74">
+        <v>91</v>
+      </c>
+      <c r="N74">
+        <v>85</v>
+      </c>
+      <c r="O74">
+        <v>87</v>
+      </c>
+      <c r="P74">
+        <v>85</v>
+      </c>
+      <c r="Q74">
+        <v>92</v>
+      </c>
+      <c r="R74">
+        <v>12</v>
+      </c>
       <c r="S74">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="T74">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="U74">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="V74">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="W74">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X74">
         <v>50</v>
       </c>
       <c r="Y74">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>86.36</v>
       </c>
       <c r="Z74">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.36</v>
       </c>
       <c r="AA74">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.76</v>
       </c>
       <c r="AB74" s="1"/>
       <c r="AC74" s="1"/>
@@ -9099,40 +9183,61 @@
       <c r="I75">
         <v>2</v>
       </c>
+      <c r="L75">
+        <v>93</v>
+      </c>
+      <c r="M75">
+        <v>84</v>
+      </c>
+      <c r="N75">
+        <v>96</v>
+      </c>
+      <c r="O75">
+        <v>81</v>
+      </c>
+      <c r="P75">
+        <v>76</v>
+      </c>
+      <c r="Q75">
+        <v>73</v>
+      </c>
+      <c r="R75">
+        <v>12</v>
+      </c>
       <c r="S75">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="T75">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="U75">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="V75">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="W75">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X75">
         <v>50</v>
       </c>
       <c r="Y75">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>88.2</v>
       </c>
       <c r="Z75">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.720000000000013</v>
       </c>
       <c r="AA75">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.960000000000008</v>
       </c>
       <c r="AB75" s="1"/>
       <c r="AC75" s="1"/>
@@ -9171,40 +9276,61 @@
       <c r="I76">
         <v>2</v>
       </c>
+      <c r="L76">
+        <v>83</v>
+      </c>
+      <c r="M76">
+        <v>94</v>
+      </c>
+      <c r="N76">
+        <v>89</v>
+      </c>
+      <c r="O76">
+        <v>86</v>
+      </c>
+      <c r="P76">
+        <v>81</v>
+      </c>
+      <c r="Q76">
+        <v>79</v>
+      </c>
+      <c r="R76">
+        <v>12</v>
+      </c>
       <c r="S76">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="T76">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="U76">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="V76">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="W76">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X76">
         <v>50</v>
       </c>
       <c r="Y76">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>87.6</v>
       </c>
       <c r="Z76">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.12</v>
       </c>
       <c r="AA76">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.84</v>
       </c>
       <c r="AB76" s="1"/>
       <c r="AC76" s="1"/>
@@ -9243,40 +9369,61 @@
       <c r="I77">
         <v>3</v>
       </c>
+      <c r="L77">
+        <v>86</v>
+      </c>
+      <c r="M77">
+        <v>86</v>
+      </c>
+      <c r="N77">
+        <v>87</v>
+      </c>
+      <c r="O77">
+        <v>84</v>
+      </c>
+      <c r="P77">
+        <v>85</v>
+      </c>
+      <c r="Q77">
+        <v>91</v>
+      </c>
+      <c r="R77">
+        <v>12</v>
+      </c>
       <c r="S77">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="T77">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="U77">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="V77">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="W77">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X77">
         <v>50</v>
       </c>
       <c r="Y77">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>86.000000000000014</v>
       </c>
       <c r="Z77">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>85.04</v>
       </c>
       <c r="AA77">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.399999999999991</v>
       </c>
       <c r="AB77" s="1"/>
       <c r="AC77" s="1"/>
@@ -9315,40 +9462,61 @@
       <c r="I78">
         <v>3</v>
       </c>
+      <c r="L78">
+        <v>80</v>
+      </c>
+      <c r="M78">
+        <v>85</v>
+      </c>
+      <c r="N78">
+        <v>81</v>
+      </c>
+      <c r="O78">
+        <v>82</v>
+      </c>
+      <c r="P78">
+        <v>88</v>
+      </c>
+      <c r="Q78">
+        <v>82</v>
+      </c>
+      <c r="R78">
+        <v>12</v>
+      </c>
       <c r="S78">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T78">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="U78">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="V78">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="W78">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X78">
         <v>50</v>
       </c>
       <c r="Y78">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>82.84</v>
       </c>
       <c r="Z78">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.16</v>
       </c>
       <c r="AA78">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>82.800000000000011</v>
       </c>
       <c r="AB78" s="1"/>
       <c r="AC78" s="1"/>
@@ -9387,40 +9555,61 @@
       <c r="I79">
         <v>3</v>
       </c>
+      <c r="L79">
+        <v>80</v>
+      </c>
+      <c r="M79">
+        <v>86</v>
+      </c>
+      <c r="N79">
+        <v>84</v>
+      </c>
+      <c r="O79">
+        <v>83</v>
+      </c>
+      <c r="P79">
+        <v>85</v>
+      </c>
+      <c r="Q79">
+        <v>78</v>
+      </c>
+      <c r="R79">
+        <v>12</v>
+      </c>
       <c r="S79">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T79">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="U79">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="V79">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="W79">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X79">
         <v>50</v>
       </c>
       <c r="Y79">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>83.440000000000012</v>
       </c>
       <c r="Z79">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.72</v>
       </c>
       <c r="AA79">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.039999999999992</v>
       </c>
       <c r="AB79" s="1"/>
       <c r="AC79" s="1"/>
@@ -9459,40 +9648,61 @@
       <c r="I80">
         <v>4</v>
       </c>
+      <c r="L80">
+        <v>76</v>
+      </c>
+      <c r="M80">
+        <v>85</v>
+      </c>
+      <c r="N80">
+        <v>88</v>
+      </c>
+      <c r="O80">
+        <v>87</v>
+      </c>
+      <c r="P80">
+        <v>93</v>
+      </c>
+      <c r="Q80">
+        <v>73</v>
+      </c>
+      <c r="R80">
+        <v>12</v>
+      </c>
       <c r="S80">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="T80">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="U80">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="V80">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="W80">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X80">
         <v>50</v>
       </c>
       <c r="Y80">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>83.760000000000019</v>
       </c>
       <c r="Z80">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>87.800000000000011</v>
       </c>
       <c r="AA80">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.16</v>
       </c>
       <c r="AB80" s="1"/>
       <c r="AC80" s="1"/>
@@ -9531,40 +9741,61 @@
       <c r="I81">
         <v>4</v>
       </c>
+      <c r="L81">
+        <v>81</v>
+      </c>
+      <c r="M81">
+        <v>89</v>
+      </c>
+      <c r="N81">
+        <v>79</v>
+      </c>
+      <c r="O81">
+        <v>81</v>
+      </c>
+      <c r="P81">
+        <v>86</v>
+      </c>
+      <c r="Q81">
+        <v>83</v>
+      </c>
+      <c r="R81">
+        <v>12</v>
+      </c>
       <c r="S81">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="T81">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="U81">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="V81">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="W81">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X81">
         <v>50</v>
       </c>
       <c r="Y81">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>83.76</v>
       </c>
       <c r="Z81">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>82.24</v>
       </c>
       <c r="AA81">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.6</v>
       </c>
       <c r="AB81" s="1"/>
       <c r="AC81" s="1"/>
@@ -9603,40 +9834,61 @@
       <c r="I82">
         <v>4</v>
       </c>
+      <c r="L82">
+        <v>92</v>
+      </c>
+      <c r="M82">
+        <v>79</v>
+      </c>
+      <c r="N82">
+        <v>85</v>
+      </c>
+      <c r="O82">
+        <v>77</v>
+      </c>
+      <c r="P82">
+        <v>74</v>
+      </c>
+      <c r="Q82">
+        <v>72</v>
+      </c>
+      <c r="R82">
+        <v>12</v>
+      </c>
       <c r="S82">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="T82">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="U82">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="V82">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="W82">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X82">
         <v>50</v>
       </c>
       <c r="Y82">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>83.679999999999993</v>
       </c>
       <c r="Z82">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>78.759999999999991</v>
       </c>
       <c r="AA82">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>82.600000000000009</v>
       </c>
       <c r="AB82" s="1"/>
       <c r="AC82" s="1"/>
@@ -9675,40 +9927,61 @@
       <c r="I83">
         <v>5</v>
       </c>
+      <c r="L83">
+        <v>80</v>
+      </c>
+      <c r="M83">
+        <v>88</v>
+      </c>
+      <c r="N83">
+        <v>94</v>
+      </c>
+      <c r="O83">
+        <v>95</v>
+      </c>
+      <c r="P83">
+        <v>87</v>
+      </c>
+      <c r="Q83">
+        <v>85</v>
+      </c>
+      <c r="R83">
+        <v>12</v>
+      </c>
       <c r="S83">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T83">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="U83">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="V83">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="W83">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X83">
         <v>50</v>
       </c>
       <c r="Y83">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>86.8</v>
       </c>
       <c r="Z83">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>92.039999999999992</v>
       </c>
       <c r="AA83">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.88</v>
       </c>
       <c r="AB83" s="1"/>
       <c r="AC83" s="1"/>
@@ -9747,40 +10020,61 @@
       <c r="I84">
         <v>5</v>
       </c>
+      <c r="L84">
+        <v>83</v>
+      </c>
+      <c r="M84">
+        <v>91</v>
+      </c>
+      <c r="N84">
+        <v>98</v>
+      </c>
+      <c r="O84">
+        <v>90</v>
+      </c>
+      <c r="P84">
+        <v>82</v>
+      </c>
+      <c r="Q84">
+        <v>76</v>
+      </c>
+      <c r="R84">
+        <v>12</v>
+      </c>
       <c r="S84">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="T84">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="U84">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="V84">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="W84">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X84">
         <v>50</v>
       </c>
       <c r="Y84">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>88.72</v>
       </c>
       <c r="Z84">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>89.800000000000011</v>
       </c>
       <c r="AA84">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>87.84</v>
       </c>
       <c r="AB84" s="1"/>
       <c r="AC84" s="1"/>
@@ -9819,40 +10113,61 @@
       <c r="I85">
         <v>6</v>
       </c>
+      <c r="L85">
+        <v>75</v>
+      </c>
+      <c r="M85">
+        <v>79</v>
+      </c>
+      <c r="N85">
+        <v>88</v>
+      </c>
+      <c r="O85">
+        <v>97</v>
+      </c>
+      <c r="P85">
+        <v>93</v>
+      </c>
+      <c r="Q85">
+        <v>77</v>
+      </c>
+      <c r="R85">
+        <v>12</v>
+      </c>
       <c r="S85">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="T85">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="U85">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="V85">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="W85">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X85">
         <v>50</v>
       </c>
       <c r="Y85">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>81.920000000000016</v>
       </c>
       <c r="Z85">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>92.080000000000013</v>
       </c>
       <c r="AA85">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>81.920000000000016</v>
       </c>
       <c r="AB85" s="1"/>
       <c r="AC85" s="1"/>
@@ -9891,40 +10206,61 @@
       <c r="I86">
         <v>6</v>
       </c>
+      <c r="L86">
+        <v>81</v>
+      </c>
+      <c r="M86">
+        <v>83</v>
+      </c>
+      <c r="N86">
+        <v>89</v>
+      </c>
+      <c r="O86">
+        <v>87</v>
+      </c>
+      <c r="P86">
+        <v>81</v>
+      </c>
+      <c r="Q86">
+        <v>78</v>
+      </c>
+      <c r="R86">
+        <v>12</v>
+      </c>
       <c r="S86">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="T86">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="U86">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="V86">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="W86">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X86">
         <v>50</v>
       </c>
       <c r="Y86">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>83.48</v>
       </c>
       <c r="Z86">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>85.64</v>
       </c>
       <c r="AA86">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.16</v>
       </c>
       <c r="AB86" s="1"/>
       <c r="AC86" s="1"/>
@@ -9963,40 +10299,61 @@
       <c r="I87">
         <v>7</v>
       </c>
+      <c r="L87">
+        <v>84</v>
+      </c>
+      <c r="M87">
+        <v>89</v>
+      </c>
+      <c r="N87">
+        <v>78</v>
+      </c>
+      <c r="O87">
+        <v>86</v>
+      </c>
+      <c r="P87">
+        <v>82</v>
+      </c>
+      <c r="Q87">
+        <v>75</v>
+      </c>
+      <c r="R87">
+        <v>12</v>
+      </c>
       <c r="S87">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="T87">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="U87">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="V87">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="W87">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X87">
         <v>50</v>
       </c>
       <c r="Y87">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>84.240000000000009</v>
       </c>
       <c r="Z87">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.760000000000019</v>
       </c>
       <c r="AA87">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>83.32</v>
       </c>
       <c r="AB87" s="1"/>
       <c r="AC87" s="1"/>
@@ -10035,40 +10392,61 @@
       <c r="I88">
         <v>7</v>
       </c>
+      <c r="L88">
+        <v>72</v>
+      </c>
+      <c r="M88">
+        <v>76</v>
+      </c>
+      <c r="N88">
+        <v>86</v>
+      </c>
+      <c r="O88">
+        <v>87</v>
+      </c>
+      <c r="P88">
+        <v>94</v>
+      </c>
+      <c r="Q88">
+        <v>70</v>
+      </c>
+      <c r="R88">
+        <v>12</v>
+      </c>
       <c r="S88">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="T88">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="U88">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="V88">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="W88">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X88">
         <v>50</v>
       </c>
       <c r="Y88">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>79.320000000000007</v>
       </c>
       <c r="Z88">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>86.720000000000013</v>
       </c>
       <c r="AA88">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="AB88" s="1"/>
       <c r="AC88" s="1"/>
@@ -10113,6 +10491,9 @@
       <c r="M89">
         <v>12</v>
       </c>
+      <c r="N89">
+        <v>95</v>
+      </c>
       <c r="O89">
         <v>12</v>
       </c>
@@ -10121,6 +10502,9 @@
       </c>
       <c r="Q89">
         <v>12</v>
+      </c>
+      <c r="R89">
+        <v>91</v>
       </c>
       <c r="S89">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
@@ -10140,22 +10524,22 @@
       </c>
       <c r="W89">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="X89">
         <v>50</v>
       </c>
       <c r="Y89">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>9.6000000000000014</v>
+        <v>28.6</v>
       </c>
       <c r="Z89">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.6000000000000014</v>
+        <v>28.6</v>
       </c>
       <c r="AA89">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.5999999999999979</v>
+        <v>28.599999999999998</v>
       </c>
       <c r="AB89" s="1"/>
       <c r="AC89" s="1"/>
@@ -10200,6 +10584,9 @@
       <c r="M90">
         <v>12</v>
       </c>
+      <c r="N90">
+        <v>75</v>
+      </c>
       <c r="O90">
         <v>12</v>
       </c>
@@ -10208,6 +10595,9 @@
       </c>
       <c r="Q90">
         <v>12</v>
+      </c>
+      <c r="R90">
+        <v>78</v>
       </c>
       <c r="S90">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
@@ -10227,22 +10617,22 @@
       </c>
       <c r="W90">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="X90">
         <v>50</v>
       </c>
       <c r="Y90">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>9.6000000000000014</v>
+        <v>24.6</v>
       </c>
       <c r="Z90">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.6000000000000014</v>
+        <v>24.6</v>
       </c>
       <c r="AA90">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>9.5999999999999979</v>
+        <v>24.599999999999998</v>
       </c>
       <c r="AB90" s="1"/>
       <c r="AC90" s="1"/>
@@ -10281,40 +10671,61 @@
       <c r="I91">
         <v>0</v>
       </c>
+      <c r="L91">
+        <v>82</v>
+      </c>
+      <c r="M91">
+        <v>82</v>
+      </c>
+      <c r="N91">
+        <v>78</v>
+      </c>
+      <c r="O91">
+        <v>79</v>
+      </c>
+      <c r="P91">
+        <v>84</v>
+      </c>
+      <c r="Q91">
+        <v>75</v>
+      </c>
+      <c r="R91">
+        <v>12</v>
+      </c>
       <c r="S91">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="T91">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="U91">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="V91">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="W91">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X91">
         <v>50</v>
       </c>
       <c r="Y91">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>81.320000000000022</v>
       </c>
       <c r="Z91">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>80.16</v>
       </c>
       <c r="AA91">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>80.760000000000019</v>
       </c>
       <c r="AB91" s="1"/>
       <c r="AC91" s="1"/>
@@ -10353,40 +10764,61 @@
       <c r="I92">
         <v>0</v>
       </c>
+      <c r="L92">
+        <v>77</v>
+      </c>
+      <c r="M92">
+        <v>83</v>
+      </c>
+      <c r="N92">
+        <v>75</v>
+      </c>
+      <c r="O92">
+        <v>79</v>
+      </c>
+      <c r="P92">
+        <v>73</v>
+      </c>
+      <c r="Q92">
+        <v>84</v>
+      </c>
+      <c r="R92">
+        <v>12</v>
+      </c>
       <c r="S92">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="T92">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="U92">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="V92">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="W92">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X92">
         <v>50</v>
       </c>
       <c r="Y92">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>78.12</v>
       </c>
       <c r="Z92">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>77.240000000000009</v>
       </c>
       <c r="AA92">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>78.440000000000012</v>
       </c>
       <c r="AB92" s="1"/>
       <c r="AC92" s="1"/>
@@ -10425,40 +10857,61 @@
       <c r="I93">
         <v>0</v>
       </c>
+      <c r="L93">
+        <v>72</v>
+      </c>
+      <c r="M93">
+        <v>68</v>
+      </c>
+      <c r="N93">
+        <v>80</v>
+      </c>
+      <c r="O93">
+        <v>84</v>
+      </c>
+      <c r="P93">
+        <v>83</v>
+      </c>
+      <c r="Q93">
+        <v>73</v>
+      </c>
+      <c r="R93">
+        <v>12</v>
+      </c>
       <c r="S93">
         <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="T93">
         <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="U93">
         <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="V93">
         <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="W93">
         <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X93">
         <v>50</v>
       </c>
       <c r="Y93">
         <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
-        <v>0</v>
+        <v>74.12</v>
       </c>
       <c r="Z93">
         <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>81.239999999999995</v>
       </c>
       <c r="AA93">
         <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
-        <v>0</v>
+        <v>74.360000000000014</v>
       </c>
       <c r="AB93" s="1"/>
       <c r="AC93" s="1"/>

</xml_diff>

<commit_message>
Added detroit red wings
</commit_message>
<xml_diff>
--- a/NHLplayers.xlsx
+++ b/NHLplayers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benca\Documents\HockeySim\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27A7C23-AA9E-4A3B-A96F-40FE9E3366EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4099CB09-7E35-42BB-8937-C9FDDEFD3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CF0E87D5-685B-476C-95EB-D2A8834F4C8B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="270">
   <si>
     <t>PlayerID</t>
   </si>
@@ -788,6 +788,138 @@
   </si>
   <si>
     <t>GameSense</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>SLO</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>D'Alessio</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>Viktor</t>
+  </si>
+  <si>
+    <t>Hämäläinen</t>
+  </si>
+  <si>
+    <t>Petterson</t>
+  </si>
+  <si>
+    <t>Lutz</t>
+  </si>
+  <si>
+    <t>Foley</t>
+  </si>
+  <si>
+    <t>Mattias</t>
+  </si>
+  <si>
+    <t>Kral</t>
+  </si>
+  <si>
+    <t>Horvat</t>
+  </si>
+  <si>
+    <t>Luka</t>
+  </si>
+  <si>
+    <t>O'Shea</t>
+  </si>
+  <si>
+    <t>Baranov</t>
+  </si>
+  <si>
+    <t>Sloane</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Kruger</t>
+  </si>
+  <si>
+    <t>Morin</t>
+  </si>
+  <si>
+    <t>Petrowski</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Jesper</t>
+  </si>
+  <si>
+    <t>Lindholm</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Aiden</t>
+  </si>
+  <si>
+    <t>Derek</t>
+  </si>
+  <si>
+    <t>Romano</t>
+  </si>
+  <si>
+    <t>Leblanc</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>Gustafsson</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Rossi</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Cody</t>
   </si>
 </sst>
 </file>
@@ -1287,9 +1419,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1375,8 +1508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{705C827B-AB13-493A-9089-0D1E20A45FF4}" name="Table1" displayName="Table1" ref="A1:AI93" totalsRowShown="0">
-  <autoFilter ref="A1:AI93" xr:uid="{705C827B-AB13-493A-9089-0D1E20A45FF4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{705C827B-AB13-493A-9089-0D1E20A45FF4}" name="Table1" displayName="Table1" ref="A1:AI116" totalsRowShown="0">
+  <autoFilter ref="A1:AI116" xr:uid="{705C827B-AB13-493A-9089-0D1E20A45FF4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA70">
     <sortCondition ref="A1:A70"/>
   </sortState>
@@ -1754,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECDA566-A1CB-4F29-BEF9-B661E32BA4DF}">
-  <dimension ref="A1:AI93"/>
+  <dimension ref="A1:AI116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G66" workbookViewId="0">
-      <selection activeCell="Y91" sqref="Y91"/>
+    <sheetView tabSelected="1" topLeftCell="J88" workbookViewId="0">
+      <selection activeCell="Y94" sqref="Y94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10922,6 +11055,2145 @@
       <c r="AH93" s="1"/>
       <c r="AI93" s="1"/>
     </row>
+    <row r="94" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" t="s">
+        <v>248</v>
+      </c>
+      <c r="D94" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" t="s">
+        <v>226</v>
+      </c>
+      <c r="F94" t="s">
+        <v>24</v>
+      </c>
+      <c r="G94" t="s">
+        <v>30</v>
+      </c>
+      <c r="H94">
+        <v>27</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>90</v>
+      </c>
+      <c r="M94">
+        <v>96</v>
+      </c>
+      <c r="N94">
+        <v>97</v>
+      </c>
+      <c r="O94">
+        <v>93</v>
+      </c>
+      <c r="P94">
+        <v>88</v>
+      </c>
+      <c r="Q94">
+        <v>99</v>
+      </c>
+      <c r="R94">
+        <v>12</v>
+      </c>
+      <c r="S94" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>90</v>
+      </c>
+      <c r="T94" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>96</v>
+      </c>
+      <c r="U94" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>93</v>
+      </c>
+      <c r="V94" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>88</v>
+      </c>
+      <c r="W94" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X94">
+        <v>50</v>
+      </c>
+      <c r="Y94" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>93.200000000000017</v>
+      </c>
+      <c r="Z94" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>92.920000000000016</v>
+      </c>
+      <c r="AA94" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>93.680000000000021</v>
+      </c>
+      <c r="AB94" s="1"/>
+      <c r="AC94" s="1"/>
+      <c r="AD94" s="1"/>
+      <c r="AE94" s="1"/>
+      <c r="AF94" s="1"/>
+      <c r="AG94" s="1"/>
+      <c r="AH94" s="1"/>
+      <c r="AI94" s="1"/>
+    </row>
+    <row r="95" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>250</v>
+      </c>
+      <c r="C95" t="s">
+        <v>251</v>
+      </c>
+      <c r="D95" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" t="s">
+        <v>226</v>
+      </c>
+      <c r="F95" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95">
+        <v>29</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>98</v>
+      </c>
+      <c r="M95">
+        <v>87</v>
+      </c>
+      <c r="N95">
+        <v>95</v>
+      </c>
+      <c r="O95">
+        <v>87</v>
+      </c>
+      <c r="P95">
+        <v>84</v>
+      </c>
+      <c r="Q95">
+        <v>78</v>
+      </c>
+      <c r="R95">
+        <v>12</v>
+      </c>
+      <c r="S95" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>98</v>
+      </c>
+      <c r="T95" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="U95" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="V95" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>84</v>
+      </c>
+      <c r="W95" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X95">
+        <v>50</v>
+      </c>
+      <c r="Y95" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>91.759999999999991</v>
+      </c>
+      <c r="Z95" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>88.44</v>
+      </c>
+      <c r="AA95" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>90.6</v>
+      </c>
+      <c r="AB95" s="1"/>
+      <c r="AC95" s="1"/>
+      <c r="AD95" s="1"/>
+      <c r="AE95" s="1"/>
+      <c r="AF95" s="1"/>
+      <c r="AG95" s="1"/>
+      <c r="AH95" s="1"/>
+      <c r="AI95" s="1"/>
+    </row>
+    <row r="96" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>252</v>
+      </c>
+      <c r="C96" t="s">
+        <v>229</v>
+      </c>
+      <c r="D96" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" t="s">
+        <v>226</v>
+      </c>
+      <c r="F96" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" t="s">
+        <v>33</v>
+      </c>
+      <c r="H96">
+        <v>25</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>89</v>
+      </c>
+      <c r="M96">
+        <v>89</v>
+      </c>
+      <c r="N96">
+        <v>87</v>
+      </c>
+      <c r="O96">
+        <v>89</v>
+      </c>
+      <c r="P96">
+        <v>92</v>
+      </c>
+      <c r="Q96">
+        <v>82</v>
+      </c>
+      <c r="R96">
+        <v>12</v>
+      </c>
+      <c r="S96" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>89</v>
+      </c>
+      <c r="T96" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>89</v>
+      </c>
+      <c r="U96" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>89</v>
+      </c>
+      <c r="V96" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>92</v>
+      </c>
+      <c r="W96" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X96">
+        <v>50</v>
+      </c>
+      <c r="Y96" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>88.960000000000008</v>
+      </c>
+      <c r="Z96" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>89.2</v>
+      </c>
+      <c r="AA96" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>88.4</v>
+      </c>
+      <c r="AB96" s="1"/>
+      <c r="AC96" s="1"/>
+      <c r="AD96" s="1"/>
+      <c r="AE96" s="1"/>
+      <c r="AF96" s="1"/>
+      <c r="AG96" s="1"/>
+      <c r="AH96" s="1"/>
+      <c r="AI96" s="1"/>
+    </row>
+    <row r="97" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" t="s">
+        <v>231</v>
+      </c>
+      <c r="D97" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" t="s">
+        <v>226</v>
+      </c>
+      <c r="F97" t="s">
+        <v>227</v>
+      </c>
+      <c r="G97" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97">
+        <v>30</v>
+      </c>
+      <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="L97">
+        <v>83</v>
+      </c>
+      <c r="M97">
+        <v>96</v>
+      </c>
+      <c r="N97">
+        <v>95</v>
+      </c>
+      <c r="O97">
+        <v>83</v>
+      </c>
+      <c r="P97">
+        <v>82</v>
+      </c>
+      <c r="Q97">
+        <v>95</v>
+      </c>
+      <c r="R97">
+        <v>12</v>
+      </c>
+      <c r="S97" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>83</v>
+      </c>
+      <c r="T97" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>96</v>
+      </c>
+      <c r="U97" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>83</v>
+      </c>
+      <c r="V97" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>82</v>
+      </c>
+      <c r="W97" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X97">
+        <v>50</v>
+      </c>
+      <c r="Y97" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>89.440000000000012</v>
+      </c>
+      <c r="Z97" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>86.24</v>
+      </c>
+      <c r="AA97" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>89.88</v>
+      </c>
+      <c r="AB97" s="1"/>
+      <c r="AC97" s="1"/>
+      <c r="AD97" s="1"/>
+      <c r="AE97" s="1"/>
+      <c r="AF97" s="1"/>
+      <c r="AG97" s="1"/>
+      <c r="AH97" s="1"/>
+      <c r="AI97" s="1"/>
+    </row>
+    <row r="98" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>253</v>
+      </c>
+      <c r="C98" t="s">
+        <v>232</v>
+      </c>
+      <c r="D98" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" t="s">
+        <v>226</v>
+      </c>
+      <c r="F98" t="s">
+        <v>24</v>
+      </c>
+      <c r="G98" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98">
+        <v>23</v>
+      </c>
+      <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="L98">
+        <v>93</v>
+      </c>
+      <c r="M98">
+        <v>80</v>
+      </c>
+      <c r="N98">
+        <v>84</v>
+      </c>
+      <c r="O98">
+        <v>81</v>
+      </c>
+      <c r="P98">
+        <v>79</v>
+      </c>
+      <c r="Q98">
+        <v>75</v>
+      </c>
+      <c r="R98">
+        <v>12</v>
+      </c>
+      <c r="S98" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>93</v>
+      </c>
+      <c r="T98" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>80</v>
+      </c>
+      <c r="U98" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>81</v>
+      </c>
+      <c r="V98" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>79</v>
+      </c>
+      <c r="W98" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X98">
+        <v>50</v>
+      </c>
+      <c r="Y98" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>84.88</v>
+      </c>
+      <c r="Z98" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>81.599999999999994</v>
+      </c>
+      <c r="AA98" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>83.96</v>
+      </c>
+      <c r="AB98" s="1"/>
+      <c r="AC98" s="1"/>
+      <c r="AD98" s="1"/>
+      <c r="AE98" s="1"/>
+      <c r="AF98" s="1"/>
+      <c r="AG98" s="1"/>
+      <c r="AH98" s="1"/>
+      <c r="AI98" s="1"/>
+    </row>
+    <row r="99" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>233</v>
+      </c>
+      <c r="C99" t="s">
+        <v>234</v>
+      </c>
+      <c r="D99" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" t="s">
+        <v>226</v>
+      </c>
+      <c r="F99" t="s">
+        <v>45</v>
+      </c>
+      <c r="G99" t="s">
+        <v>30</v>
+      </c>
+      <c r="H99">
+        <v>26</v>
+      </c>
+      <c r="I99">
+        <v>2</v>
+      </c>
+      <c r="L99">
+        <v>87</v>
+      </c>
+      <c r="M99">
+        <v>85</v>
+      </c>
+      <c r="N99">
+        <v>84</v>
+      </c>
+      <c r="O99">
+        <v>87</v>
+      </c>
+      <c r="P99">
+        <v>86</v>
+      </c>
+      <c r="Q99">
+        <v>82</v>
+      </c>
+      <c r="R99">
+        <v>12</v>
+      </c>
+      <c r="S99" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="T99" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="U99" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="V99" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>86</v>
+      </c>
+      <c r="W99" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X99">
+        <v>50</v>
+      </c>
+      <c r="Y99" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>85.64</v>
+      </c>
+      <c r="Z99" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>86.039999999999992</v>
+      </c>
+      <c r="AA99" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>85.320000000000007</v>
+      </c>
+      <c r="AB99" s="1"/>
+      <c r="AC99" s="1"/>
+      <c r="AD99" s="1"/>
+      <c r="AE99" s="1"/>
+      <c r="AF99" s="1"/>
+      <c r="AG99" s="1"/>
+      <c r="AH99" s="1"/>
+      <c r="AI99" s="1"/>
+    </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>254</v>
+      </c>
+      <c r="C100" t="s">
+        <v>255</v>
+      </c>
+      <c r="D100" t="s">
+        <v>23</v>
+      </c>
+      <c r="E100" t="s">
+        <v>226</v>
+      </c>
+      <c r="F100" t="s">
+        <v>19</v>
+      </c>
+      <c r="G100" t="s">
+        <v>30</v>
+      </c>
+      <c r="H100">
+        <v>28</v>
+      </c>
+      <c r="I100">
+        <v>3</v>
+      </c>
+      <c r="L100">
+        <v>85</v>
+      </c>
+      <c r="M100">
+        <v>86</v>
+      </c>
+      <c r="N100">
+        <v>89</v>
+      </c>
+      <c r="O100">
+        <v>86</v>
+      </c>
+      <c r="P100">
+        <v>84</v>
+      </c>
+      <c r="Q100">
+        <v>89</v>
+      </c>
+      <c r="R100">
+        <v>12</v>
+      </c>
+      <c r="S100" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="T100" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>86</v>
+      </c>
+      <c r="U100" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>86</v>
+      </c>
+      <c r="V100" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>84</v>
+      </c>
+      <c r="W100" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X100">
+        <v>50</v>
+      </c>
+      <c r="Y100" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>86.039999999999992</v>
+      </c>
+      <c r="Z100" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>86.16</v>
+      </c>
+      <c r="AA100" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>86.32</v>
+      </c>
+      <c r="AB100" s="1"/>
+      <c r="AC100" s="1"/>
+      <c r="AD100" s="1"/>
+      <c r="AE100" s="1"/>
+      <c r="AF100" s="1"/>
+      <c r="AG100" s="1"/>
+      <c r="AH100" s="1"/>
+      <c r="AI100" s="1"/>
+    </row>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" t="s">
+        <v>235</v>
+      </c>
+      <c r="D101" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101" t="s">
+        <v>226</v>
+      </c>
+      <c r="F101" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" t="s">
+        <v>25</v>
+      </c>
+      <c r="H101">
+        <v>24</v>
+      </c>
+      <c r="I101">
+        <v>3</v>
+      </c>
+      <c r="L101">
+        <v>81</v>
+      </c>
+      <c r="M101">
+        <v>88</v>
+      </c>
+      <c r="N101">
+        <v>85</v>
+      </c>
+      <c r="O101">
+        <v>80</v>
+      </c>
+      <c r="P101">
+        <v>77</v>
+      </c>
+      <c r="Q101">
+        <v>74</v>
+      </c>
+      <c r="R101">
+        <v>12</v>
+      </c>
+      <c r="S101" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>81</v>
+      </c>
+      <c r="T101" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>88</v>
+      </c>
+      <c r="U101" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>80</v>
+      </c>
+      <c r="V101" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="W101" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X101">
+        <v>50</v>
+      </c>
+      <c r="Y101" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>83.52000000000001</v>
+      </c>
+      <c r="Z101" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>81.08</v>
+      </c>
+      <c r="AA101" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.68</v>
+      </c>
+      <c r="AB101" s="1"/>
+      <c r="AC101" s="1"/>
+      <c r="AD101" s="1"/>
+      <c r="AE101" s="1"/>
+      <c r="AF101" s="1"/>
+      <c r="AG101" s="1"/>
+      <c r="AH101" s="1"/>
+      <c r="AI101" s="1"/>
+    </row>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102" t="s">
+        <v>256</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" t="s">
+        <v>226</v>
+      </c>
+      <c r="F102" t="s">
+        <v>24</v>
+      </c>
+      <c r="G102" t="s">
+        <v>33</v>
+      </c>
+      <c r="H102">
+        <v>32</v>
+      </c>
+      <c r="I102">
+        <v>3</v>
+      </c>
+      <c r="L102">
+        <v>77</v>
+      </c>
+      <c r="M102">
+        <v>82</v>
+      </c>
+      <c r="N102">
+        <v>92</v>
+      </c>
+      <c r="O102">
+        <v>81</v>
+      </c>
+      <c r="P102">
+        <v>87</v>
+      </c>
+      <c r="Q102">
+        <v>79</v>
+      </c>
+      <c r="R102">
+        <v>12</v>
+      </c>
+      <c r="S102" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="T102" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>82</v>
+      </c>
+      <c r="U102" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>81</v>
+      </c>
+      <c r="V102" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="W102" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X102">
+        <v>50</v>
+      </c>
+      <c r="Y102" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>82.960000000000008</v>
+      </c>
+      <c r="Z102" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>84.320000000000007</v>
+      </c>
+      <c r="AA102" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.920000000000016</v>
+      </c>
+      <c r="AB102" s="1"/>
+      <c r="AC102" s="1"/>
+      <c r="AD102" s="1"/>
+      <c r="AE102" s="1"/>
+      <c r="AF102" s="1"/>
+      <c r="AG102" s="1"/>
+      <c r="AH102" s="1"/>
+      <c r="AI102" s="1"/>
+    </row>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" t="s">
+        <v>236</v>
+      </c>
+      <c r="D103" t="s">
+        <v>23</v>
+      </c>
+      <c r="E103" t="s">
+        <v>226</v>
+      </c>
+      <c r="F103" t="s">
+        <v>51</v>
+      </c>
+      <c r="G103" t="s">
+        <v>30</v>
+      </c>
+      <c r="H103">
+        <v>22</v>
+      </c>
+      <c r="I103">
+        <v>4</v>
+      </c>
+      <c r="L103">
+        <v>81</v>
+      </c>
+      <c r="M103">
+        <v>83</v>
+      </c>
+      <c r="N103">
+        <v>78</v>
+      </c>
+      <c r="O103">
+        <v>83</v>
+      </c>
+      <c r="P103">
+        <v>85</v>
+      </c>
+      <c r="Q103">
+        <v>88</v>
+      </c>
+      <c r="R103">
+        <v>12</v>
+      </c>
+      <c r="S103" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>81</v>
+      </c>
+      <c r="T103" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>83</v>
+      </c>
+      <c r="U103" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>83</v>
+      </c>
+      <c r="V103" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="W103" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X103">
+        <v>50</v>
+      </c>
+      <c r="Y103" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>81.600000000000023</v>
+      </c>
+      <c r="Z103" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.320000000000022</v>
+      </c>
+      <c r="AA103" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.080000000000013</v>
+      </c>
+      <c r="AB103" s="1"/>
+      <c r="AC103" s="1"/>
+      <c r="AD103" s="1"/>
+      <c r="AE103" s="1"/>
+      <c r="AF103" s="1"/>
+      <c r="AG103" s="1"/>
+      <c r="AH103" s="1"/>
+      <c r="AI103" s="1"/>
+    </row>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>257</v>
+      </c>
+      <c r="C104" t="s">
+        <v>237</v>
+      </c>
+      <c r="D104" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" t="s">
+        <v>226</v>
+      </c>
+      <c r="F104" t="s">
+        <v>19</v>
+      </c>
+      <c r="G104" t="s">
+        <v>48</v>
+      </c>
+      <c r="H104">
+        <v>34</v>
+      </c>
+      <c r="I104">
+        <v>4</v>
+      </c>
+      <c r="L104">
+        <v>79</v>
+      </c>
+      <c r="M104">
+        <v>76</v>
+      </c>
+      <c r="N104">
+        <v>89</v>
+      </c>
+      <c r="O104">
+        <v>80</v>
+      </c>
+      <c r="P104">
+        <v>94</v>
+      </c>
+      <c r="Q104">
+        <v>73</v>
+      </c>
+      <c r="R104">
+        <v>12</v>
+      </c>
+      <c r="S104" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>79</v>
+      </c>
+      <c r="T104" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>76</v>
+      </c>
+      <c r="U104" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>80</v>
+      </c>
+      <c r="V104" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>94</v>
+      </c>
+      <c r="W104" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X104">
+        <v>50</v>
+      </c>
+      <c r="Y104" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>81.88</v>
+      </c>
+      <c r="Z104" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>84.24</v>
+      </c>
+      <c r="AA104" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>81.52</v>
+      </c>
+      <c r="AB104" s="1"/>
+      <c r="AC104" s="1"/>
+      <c r="AD104" s="1"/>
+      <c r="AE104" s="1"/>
+      <c r="AF104" s="1"/>
+      <c r="AG104" s="1"/>
+      <c r="AH104" s="1"/>
+      <c r="AI104" s="1"/>
+    </row>
+    <row r="105" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>258</v>
+      </c>
+      <c r="C105" t="s">
+        <v>259</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" t="s">
+        <v>226</v>
+      </c>
+      <c r="F105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G105" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105">
+        <v>25</v>
+      </c>
+      <c r="I105">
+        <v>4</v>
+      </c>
+      <c r="L105">
+        <v>82</v>
+      </c>
+      <c r="M105">
+        <v>87</v>
+      </c>
+      <c r="N105">
+        <v>85</v>
+      </c>
+      <c r="O105">
+        <v>77</v>
+      </c>
+      <c r="P105">
+        <v>79</v>
+      </c>
+      <c r="Q105">
+        <v>72</v>
+      </c>
+      <c r="R105">
+        <v>12</v>
+      </c>
+      <c r="S105" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>82</v>
+      </c>
+      <c r="T105" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="U105" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="V105" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>79</v>
+      </c>
+      <c r="W105" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X105">
+        <v>50</v>
+      </c>
+      <c r="Y105" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>83.64</v>
+      </c>
+      <c r="Z105" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>80</v>
+      </c>
+      <c r="AA105" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.64</v>
+      </c>
+      <c r="AB105" s="1"/>
+      <c r="AC105" s="1"/>
+      <c r="AD105" s="1"/>
+      <c r="AE105" s="1"/>
+      <c r="AF105" s="1"/>
+      <c r="AG105" s="1"/>
+      <c r="AH105" s="1"/>
+      <c r="AI105" s="1"/>
+    </row>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>238</v>
+      </c>
+      <c r="C106" t="s">
+        <v>260</v>
+      </c>
+      <c r="D106" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" t="s">
+        <v>226</v>
+      </c>
+      <c r="F106" t="s">
+        <v>29</v>
+      </c>
+      <c r="G106" t="s">
+        <v>61</v>
+      </c>
+      <c r="H106">
+        <v>29</v>
+      </c>
+      <c r="I106">
+        <v>5</v>
+      </c>
+      <c r="L106">
+        <v>85</v>
+      </c>
+      <c r="M106">
+        <v>88</v>
+      </c>
+      <c r="N106">
+        <v>95</v>
+      </c>
+      <c r="O106">
+        <v>91</v>
+      </c>
+      <c r="P106">
+        <v>85</v>
+      </c>
+      <c r="Q106">
+        <v>80</v>
+      </c>
+      <c r="R106">
+        <v>12</v>
+      </c>
+      <c r="S106" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="T106" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>88</v>
+      </c>
+      <c r="U106" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>91</v>
+      </c>
+      <c r="V106" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="W106" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X106">
+        <v>50</v>
+      </c>
+      <c r="Y106" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>88.2</v>
+      </c>
+      <c r="Z106" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>90.12</v>
+      </c>
+      <c r="AA106" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>87.679999999999993</v>
+      </c>
+      <c r="AB106" s="1"/>
+      <c r="AC106" s="1"/>
+      <c r="AD106" s="1"/>
+      <c r="AE106" s="1"/>
+      <c r="AF106" s="1"/>
+      <c r="AG106" s="1"/>
+      <c r="AH106" s="1"/>
+      <c r="AI106" s="1"/>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>262</v>
+      </c>
+      <c r="C107" t="s">
+        <v>261</v>
+      </c>
+      <c r="D107" t="s">
+        <v>60</v>
+      </c>
+      <c r="E107" t="s">
+        <v>226</v>
+      </c>
+      <c r="F107" t="s">
+        <v>24</v>
+      </c>
+      <c r="G107" t="s">
+        <v>57</v>
+      </c>
+      <c r="H107">
+        <v>27</v>
+      </c>
+      <c r="I107">
+        <v>5</v>
+      </c>
+      <c r="L107">
+        <v>78</v>
+      </c>
+      <c r="M107">
+        <v>85</v>
+      </c>
+      <c r="N107">
+        <v>95</v>
+      </c>
+      <c r="O107">
+        <v>94</v>
+      </c>
+      <c r="P107">
+        <v>90</v>
+      </c>
+      <c r="Q107">
+        <v>79</v>
+      </c>
+      <c r="R107">
+        <v>12</v>
+      </c>
+      <c r="S107" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>78</v>
+      </c>
+      <c r="T107" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="U107" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>94</v>
+      </c>
+      <c r="V107" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>90</v>
+      </c>
+      <c r="W107" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X107">
+        <v>50</v>
+      </c>
+      <c r="Y107" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>85.720000000000013</v>
+      </c>
+      <c r="Z107" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>92.04</v>
+      </c>
+      <c r="AA107" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>85.52000000000001</v>
+      </c>
+      <c r="AB107" s="1"/>
+      <c r="AC107" s="1"/>
+      <c r="AD107" s="1"/>
+      <c r="AE107" s="1"/>
+      <c r="AF107" s="1"/>
+      <c r="AG107" s="1"/>
+      <c r="AH107" s="1"/>
+      <c r="AI107" s="1"/>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>263</v>
+      </c>
+      <c r="C108" t="s">
+        <v>239</v>
+      </c>
+      <c r="D108" t="s">
+        <v>56</v>
+      </c>
+      <c r="E108" t="s">
+        <v>226</v>
+      </c>
+      <c r="F108" t="s">
+        <v>38</v>
+      </c>
+      <c r="G108" t="s">
+        <v>67</v>
+      </c>
+      <c r="H108">
+        <v>25</v>
+      </c>
+      <c r="I108">
+        <v>6</v>
+      </c>
+      <c r="L108">
+        <v>76</v>
+      </c>
+      <c r="M108">
+        <v>79</v>
+      </c>
+      <c r="N108">
+        <v>90</v>
+      </c>
+      <c r="O108">
+        <v>92</v>
+      </c>
+      <c r="P108">
+        <v>91</v>
+      </c>
+      <c r="Q108">
+        <v>77</v>
+      </c>
+      <c r="R108">
+        <v>12</v>
+      </c>
+      <c r="S108" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>76</v>
+      </c>
+      <c r="T108" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>79</v>
+      </c>
+      <c r="U108" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>92</v>
+      </c>
+      <c r="V108" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>91</v>
+      </c>
+      <c r="W108" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X108">
+        <v>50</v>
+      </c>
+      <c r="Y108" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>82.2</v>
+      </c>
+      <c r="Z108" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>89.72</v>
+      </c>
+      <c r="AA108" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>82.160000000000011</v>
+      </c>
+      <c r="AB108" s="1"/>
+      <c r="AC108" s="1"/>
+      <c r="AD108" s="1"/>
+      <c r="AE108" s="1"/>
+      <c r="AF108" s="1"/>
+      <c r="AG108" s="1"/>
+      <c r="AH108" s="1"/>
+      <c r="AI108" s="1"/>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>264</v>
+      </c>
+      <c r="C109" t="s">
+        <v>265</v>
+      </c>
+      <c r="D109" t="s">
+        <v>60</v>
+      </c>
+      <c r="E109" t="s">
+        <v>226</v>
+      </c>
+      <c r="F109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G109" t="s">
+        <v>57</v>
+      </c>
+      <c r="H109">
+        <v>31</v>
+      </c>
+      <c r="I109">
+        <v>6</v>
+      </c>
+      <c r="L109">
+        <v>77</v>
+      </c>
+      <c r="M109">
+        <v>80</v>
+      </c>
+      <c r="N109">
+        <v>95</v>
+      </c>
+      <c r="O109">
+        <v>89</v>
+      </c>
+      <c r="P109">
+        <v>89</v>
+      </c>
+      <c r="Q109">
+        <v>77</v>
+      </c>
+      <c r="R109">
+        <v>12</v>
+      </c>
+      <c r="S109" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="T109" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>80</v>
+      </c>
+      <c r="U109" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>89</v>
+      </c>
+      <c r="V109" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>89</v>
+      </c>
+      <c r="W109" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X109">
+        <v>50</v>
+      </c>
+      <c r="Y109" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>83.48</v>
+      </c>
+      <c r="Z109" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>89</v>
+      </c>
+      <c r="AA109" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>83.36</v>
+      </c>
+      <c r="AB109" s="1"/>
+      <c r="AC109" s="1"/>
+      <c r="AD109" s="1"/>
+      <c r="AE109" s="1"/>
+      <c r="AF109" s="1"/>
+      <c r="AG109" s="1"/>
+      <c r="AH109" s="1"/>
+      <c r="AI109" s="1"/>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>241</v>
+      </c>
+      <c r="C110" t="s">
+        <v>240</v>
+      </c>
+      <c r="D110" t="s">
+        <v>56</v>
+      </c>
+      <c r="E110" t="s">
+        <v>226</v>
+      </c>
+      <c r="F110" t="s">
+        <v>228</v>
+      </c>
+      <c r="G110" t="s">
+        <v>61</v>
+      </c>
+      <c r="H110">
+        <v>23</v>
+      </c>
+      <c r="I110">
+        <v>7</v>
+      </c>
+      <c r="L110">
+        <v>79</v>
+      </c>
+      <c r="M110">
+        <v>85</v>
+      </c>
+      <c r="N110">
+        <v>79</v>
+      </c>
+      <c r="O110">
+        <v>86</v>
+      </c>
+      <c r="P110">
+        <v>84</v>
+      </c>
+      <c r="Q110">
+        <v>72</v>
+      </c>
+      <c r="R110">
+        <v>12</v>
+      </c>
+      <c r="S110" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>79</v>
+      </c>
+      <c r="T110" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>85</v>
+      </c>
+      <c r="U110" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>86</v>
+      </c>
+      <c r="V110" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>84</v>
+      </c>
+      <c r="W110" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X110">
+        <v>50</v>
+      </c>
+      <c r="Y110" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>81.8</v>
+      </c>
+      <c r="Z110" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>83.84</v>
+      </c>
+      <c r="AA110" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>81</v>
+      </c>
+      <c r="AB110" s="1"/>
+      <c r="AC110" s="1"/>
+      <c r="AD110" s="1"/>
+      <c r="AE110" s="1"/>
+      <c r="AF110" s="1"/>
+      <c r="AG110" s="1"/>
+      <c r="AH110" s="1"/>
+      <c r="AI110" s="1"/>
+    </row>
+    <row r="111" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>266</v>
+      </c>
+      <c r="C111" t="s">
+        <v>242</v>
+      </c>
+      <c r="D111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E111" t="s">
+        <v>226</v>
+      </c>
+      <c r="F111" t="s">
+        <v>24</v>
+      </c>
+      <c r="G111" t="s">
+        <v>67</v>
+      </c>
+      <c r="H111">
+        <v>34</v>
+      </c>
+      <c r="I111">
+        <v>7</v>
+      </c>
+      <c r="L111">
+        <v>70</v>
+      </c>
+      <c r="M111">
+        <v>75</v>
+      </c>
+      <c r="N111">
+        <v>87</v>
+      </c>
+      <c r="O111">
+        <v>87</v>
+      </c>
+      <c r="P111">
+        <v>95</v>
+      </c>
+      <c r="Q111">
+        <v>67</v>
+      </c>
+      <c r="R111">
+        <v>12</v>
+      </c>
+      <c r="S111" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>70</v>
+      </c>
+      <c r="T111" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>75</v>
+      </c>
+      <c r="U111" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="V111" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>95</v>
+      </c>
+      <c r="W111" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X111">
+        <v>50</v>
+      </c>
+      <c r="Y111" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>78.680000000000007</v>
+      </c>
+      <c r="Z111" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>86.96</v>
+      </c>
+      <c r="AA111" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>78.240000000000009</v>
+      </c>
+      <c r="AB111" s="1"/>
+      <c r="AC111" s="1"/>
+      <c r="AD111" s="1"/>
+      <c r="AE111" s="1"/>
+      <c r="AF111" s="1"/>
+      <c r="AG111" s="1"/>
+      <c r="AH111" s="1"/>
+      <c r="AI111" s="1"/>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>267</v>
+      </c>
+      <c r="C112" t="s">
+        <v>243</v>
+      </c>
+      <c r="D112" t="s">
+        <v>74</v>
+      </c>
+      <c r="E112" t="s">
+        <v>226</v>
+      </c>
+      <c r="F112" t="s">
+        <v>66</v>
+      </c>
+      <c r="G112" t="s">
+        <v>75</v>
+      </c>
+      <c r="H112">
+        <v>28</v>
+      </c>
+      <c r="I112">
+        <v>8</v>
+      </c>
+      <c r="L112">
+        <v>12</v>
+      </c>
+      <c r="M112">
+        <v>12</v>
+      </c>
+      <c r="N112">
+        <v>12</v>
+      </c>
+      <c r="O112">
+        <v>12</v>
+      </c>
+      <c r="P112">
+        <v>12</v>
+      </c>
+      <c r="Q112">
+        <v>12</v>
+      </c>
+      <c r="R112">
+        <v>88</v>
+      </c>
+      <c r="S112" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="T112" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="U112" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="V112" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="W112" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>88</v>
+      </c>
+      <c r="X112">
+        <v>50</v>
+      </c>
+      <c r="Y112" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>12.000000000000002</v>
+      </c>
+      <c r="Z112" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>12.000000000000002</v>
+      </c>
+      <c r="AA112" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>11.999999999999998</v>
+      </c>
+      <c r="AB112" s="1"/>
+      <c r="AC112" s="1"/>
+      <c r="AD112" s="1"/>
+      <c r="AE112" s="1"/>
+      <c r="AF112" s="1"/>
+      <c r="AG112" s="1"/>
+      <c r="AH112" s="1"/>
+      <c r="AI112" s="1"/>
+    </row>
+    <row r="113" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>245</v>
+      </c>
+      <c r="C113" t="s">
+        <v>244</v>
+      </c>
+      <c r="D113" t="s">
+        <v>74</v>
+      </c>
+      <c r="E113" t="s">
+        <v>226</v>
+      </c>
+      <c r="F113" t="s">
+        <v>19</v>
+      </c>
+      <c r="G113" t="s">
+        <v>75</v>
+      </c>
+      <c r="H113">
+        <v>23</v>
+      </c>
+      <c r="I113">
+        <v>9</v>
+      </c>
+      <c r="L113">
+        <v>12</v>
+      </c>
+      <c r="M113">
+        <v>12</v>
+      </c>
+      <c r="N113">
+        <v>12</v>
+      </c>
+      <c r="O113">
+        <v>12</v>
+      </c>
+      <c r="P113">
+        <v>12</v>
+      </c>
+      <c r="Q113">
+        <v>12</v>
+      </c>
+      <c r="R113">
+        <v>80</v>
+      </c>
+      <c r="S113" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="T113" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="U113" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="V113" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="W113" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>80</v>
+      </c>
+      <c r="X113">
+        <v>50</v>
+      </c>
+      <c r="Y113" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>12.000000000000002</v>
+      </c>
+      <c r="Z113" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>12.000000000000002</v>
+      </c>
+      <c r="AA113" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>11.999999999999998</v>
+      </c>
+      <c r="AB113" s="1"/>
+      <c r="AC113" s="1"/>
+      <c r="AD113" s="1"/>
+      <c r="AE113" s="1"/>
+      <c r="AF113" s="1"/>
+      <c r="AG113" s="1"/>
+      <c r="AH113" s="1"/>
+      <c r="AI113" s="1"/>
+    </row>
+    <row r="114" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>268</v>
+      </c>
+      <c r="C114" t="s">
+        <v>246</v>
+      </c>
+      <c r="D114" t="s">
+        <v>56</v>
+      </c>
+      <c r="E114" t="s">
+        <v>226</v>
+      </c>
+      <c r="F114" t="s">
+        <v>29</v>
+      </c>
+      <c r="G114" t="s">
+        <v>57</v>
+      </c>
+      <c r="H114">
+        <v>24</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>78</v>
+      </c>
+      <c r="M114">
+        <v>77</v>
+      </c>
+      <c r="N114">
+        <v>79</v>
+      </c>
+      <c r="O114">
+        <v>83</v>
+      </c>
+      <c r="P114">
+        <v>84</v>
+      </c>
+      <c r="Q114">
+        <v>76</v>
+      </c>
+      <c r="R114">
+        <v>12</v>
+      </c>
+      <c r="S114" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>78</v>
+      </c>
+      <c r="T114" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="U114" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>83</v>
+      </c>
+      <c r="V114" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>84</v>
+      </c>
+      <c r="W114" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X114">
+        <v>50</v>
+      </c>
+      <c r="Y114" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>78.8</v>
+      </c>
+      <c r="Z114" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>81.72</v>
+      </c>
+      <c r="AA114" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>78.679999999999993</v>
+      </c>
+      <c r="AB114" s="1"/>
+      <c r="AC114" s="1"/>
+      <c r="AD114" s="1"/>
+      <c r="AE114" s="1"/>
+      <c r="AF114" s="1"/>
+      <c r="AG114" s="1"/>
+      <c r="AH114" s="1"/>
+      <c r="AI114" s="1"/>
+    </row>
+    <row r="115" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>269</v>
+      </c>
+      <c r="C115" t="s">
+        <v>247</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" t="s">
+        <v>226</v>
+      </c>
+      <c r="F115" t="s">
+        <v>24</v>
+      </c>
+      <c r="G115" t="s">
+        <v>20</v>
+      </c>
+      <c r="H115">
+        <v>21</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>87</v>
+      </c>
+      <c r="M115">
+        <v>74</v>
+      </c>
+      <c r="N115">
+        <v>71</v>
+      </c>
+      <c r="O115">
+        <v>72</v>
+      </c>
+      <c r="P115">
+        <v>74</v>
+      </c>
+      <c r="Q115">
+        <v>74</v>
+      </c>
+      <c r="R115">
+        <v>12</v>
+      </c>
+      <c r="S115" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>87</v>
+      </c>
+      <c r="T115" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>74</v>
+      </c>
+      <c r="U115" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>72</v>
+      </c>
+      <c r="V115" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>74</v>
+      </c>
+      <c r="W115" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X115">
+        <v>50</v>
+      </c>
+      <c r="Y115" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>77.48</v>
+      </c>
+      <c r="Z115" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>72.959999999999994</v>
+      </c>
+      <c r="AA115" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>76.960000000000008</v>
+      </c>
+      <c r="AB115" s="1"/>
+      <c r="AC115" s="1"/>
+      <c r="AD115" s="1"/>
+      <c r="AE115" s="1"/>
+      <c r="AF115" s="1"/>
+      <c r="AG115" s="1"/>
+      <c r="AH115" s="1"/>
+      <c r="AI115" s="1"/>
+    </row>
+    <row r="116" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>54</v>
+      </c>
+      <c r="C116" t="s">
+        <v>152</v>
+      </c>
+      <c r="D116" t="s">
+        <v>23</v>
+      </c>
+      <c r="E116" t="s">
+        <v>226</v>
+      </c>
+      <c r="F116" t="s">
+        <v>19</v>
+      </c>
+      <c r="G116" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116">
+        <v>29</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>75</v>
+      </c>
+      <c r="M116">
+        <v>84</v>
+      </c>
+      <c r="N116">
+        <v>82</v>
+      </c>
+      <c r="O116">
+        <v>77</v>
+      </c>
+      <c r="P116">
+        <v>77</v>
+      </c>
+      <c r="Q116">
+        <v>85</v>
+      </c>
+      <c r="R116">
+        <v>12</v>
+      </c>
+      <c r="S116" s="2">
+        <f>Table1[[#This Row],[Shooting]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>75</v>
+      </c>
+      <c r="T116" s="2">
+        <f>Table1[[#This Row],[Playmaking]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>84</v>
+      </c>
+      <c r="U116" s="2">
+        <f>Table1[[#This Row],[Defense]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="V116" s="2">
+        <f>Table1[[#This Row],[Physicality]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>77</v>
+      </c>
+      <c r="W116" s="2">
+        <f>Table1[[#This Row],[Goaltend]]*(1.5^((0.01*(50+Table1[[#This Row],[Morale]]))-1))</f>
+        <v>12</v>
+      </c>
+      <c r="X116">
+        <v>50</v>
+      </c>
+      <c r="Y116" s="2">
+        <f>(0.4*(Table1[[#This Row],[M_Shooting]]+Table1[[#This Row],[M_Playmaking]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*(Table1[[#This Row],[M_Physicality]]))*0.8+(Table1[[#This Row],[GameSense]]*0.2)</f>
+        <v>79.600000000000009</v>
+      </c>
+      <c r="Z116" s="2">
+        <f>(0.05*(Table1[[#This Row],[M_Shooting]])+0.1*(Table1[[#This Row],[M_Playmaking]])+0.6*Table1[[#This Row],[M_Defense]]+0.25*Table1[[#This Row],[M_Physicality]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>78.48</v>
+      </c>
+      <c r="AA116" s="2">
+        <f>(0.35*(Table1[[#This Row],[M_Playmaking]]+Table1[[#This Row],[M_Shooting]])+0.05*(Table1[[#This Row],[M_Defense]])+0.15*Table1[[#This Row],[M_Physicality]]+0.1*Table1[[#This Row],[Faceoff]])*0.8+(0.2*Table1[[#This Row],[GameSense]])</f>
+        <v>80.040000000000006</v>
+      </c>
+      <c r="AB116" s="1"/>
+      <c r="AC116" s="1"/>
+      <c r="AD116" s="1"/>
+      <c r="AE116" s="1"/>
+      <c r="AF116" s="1"/>
+      <c r="AG116" s="1"/>
+      <c r="AH116" s="1"/>
+      <c r="AI116" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>